<commit_message>
add DDL file update ini file add sql stuff
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\el_du\source\repos\ETLDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7803BFE8-5F6A-48E2-AD9E-E5A977080296}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032C79CE-8F34-468B-84F8-B2924726CEEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23730" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{3D9D8036-FB6C-44AE-99B6-1C9335697817}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{3D9D8036-FB6C-44AE-99B6-1C9335697817}"/>
   </bookViews>
   <sheets>
     <sheet name="Github" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>date</t>
   </si>
   <si>
-    <t>US</t>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>